<commit_message>
[+] CF raw SQL
</commit_message>
<xml_diff>
--- a/_results/RawResults-02-with-linq2db.xlsx
+++ b/_results/RawResults-02-with-linq2db.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>simple CF/10</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>simple BLT raw/500</t>
+  </si>
+  <si>
+    <t>simple CF raw/10</t>
+  </si>
+  <si>
+    <t>simple CF raw/500</t>
+  </si>
+  <si>
+    <t>complex CF raw/10</t>
+  </si>
+  <si>
+    <t>complex CF raw/500</t>
+  </si>
+  <si>
+    <t>s CF raw/10+10</t>
   </si>
 </sst>
 </file>
@@ -459,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I29"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,29 +523,29 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>851</v>
+        <v>829</v>
       </c>
       <c r="D5">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E5">
-        <v>851</v>
+        <v>862</v>
       </c>
       <c r="F5" s="1">
         <f>(C5+D5+E5)/3</f>
-        <v>855</v>
+        <v>850.33333333333337</v>
       </c>
       <c r="G5">
         <f>F5/1000</f>
-        <v>0.85499999999999998</v>
+        <v>0.85033333333333339</v>
       </c>
       <c r="H5" s="2">
-        <f>$H$25</f>
-        <v>0.22633333333333328</v>
+        <f>$H$29</f>
+        <v>0.22466666666666679</v>
       </c>
       <c r="I5">
         <f>G5-H5</f>
-        <v>0.62866666666666671</v>
+        <v>0.62566666666666659</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -538,699 +553,845 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2084</v>
+        <v>2114</v>
       </c>
       <c r="D6">
-        <v>2103</v>
+        <v>2083</v>
       </c>
       <c r="E6">
-        <v>2077</v>
+        <v>2082</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F29" si="0">(C6+D6+E6)/3</f>
-        <v>2088</v>
+        <f t="shared" ref="F6:F34" si="0">(C6+D6+E6)/3</f>
+        <v>2093</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G29" si="1">F6/1000</f>
-        <v>2.0880000000000001</v>
+        <f t="shared" ref="G6:G34" si="1">F6/1000</f>
+        <v>2.093</v>
       </c>
       <c r="H6" s="2">
-        <f>$H$25</f>
-        <v>0.22633333333333328</v>
+        <f>$H$29</f>
+        <v>0.22466666666666679</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I24" si="2">G6-H6</f>
-        <v>1.8616666666666668</v>
+        <f t="shared" ref="I6:I28" si="2">G6-H6</f>
+        <v>1.8683333333333332</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>141</v>
+        <v>364</v>
       </c>
       <c r="D7">
-        <v>153</v>
+        <v>375</v>
       </c>
       <c r="E7">
-        <v>135</v>
+        <v>397</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>143</v>
+        <v>378.66666666666669</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>0.14299999999999999</v>
+        <v>0.37866666666666671</v>
       </c>
       <c r="H7" s="2">
-        <f>$H$26</f>
-        <v>4.2333333333333306E-2</v>
+        <f>$H$30</f>
+        <v>0.13666666666666683</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>0.10066666666666668</v>
+        <v>0.24199999999999988</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>1119</v>
+        <v>1508</v>
       </c>
       <c r="D8">
-        <v>1104</v>
+        <v>1451</v>
       </c>
       <c r="E8">
-        <v>1145</v>
+        <v>1418</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>1122.6666666666667</v>
+        <v>1459</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>1.1226666666666667</v>
+        <v>1.4590000000000001</v>
       </c>
       <c r="H8" s="2">
-        <f>$H$26</f>
-        <v>4.2333333333333306E-2</v>
+        <f>$H$30</f>
+        <v>0.13666666666666683</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>1.0803333333333334</v>
+        <v>1.3223333333333334</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>183</v>
+        <v>136</v>
       </c>
       <c r="D9">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="E9">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>175.66666666666666</v>
+        <v>142.66666666666666</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>0.17566666666666667</v>
+        <v>0.14266666666666666</v>
       </c>
       <c r="H9" s="2">
-        <f>$H$27</f>
-        <v>5.5999999999999994E-2</v>
+        <f>$H$31</f>
+        <v>4.6666666666666662E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>0.11966666666666667</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>1391</v>
+        <v>1126</v>
       </c>
       <c r="D10">
-        <v>1366</v>
+        <v>1126</v>
       </c>
       <c r="E10">
-        <v>1378</v>
+        <v>1125</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>1378.3333333333333</v>
+        <v>1125.6666666666667</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>1.3783333333333332</v>
+        <v>1.1256666666666668</v>
       </c>
       <c r="H10" s="2">
-        <f>$H$27</f>
-        <v>5.5999999999999994E-2</v>
+        <f>$H$31</f>
+        <v>4.6666666666666662E-2</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>1.3223333333333331</v>
+        <v>1.0790000000000002</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="D11">
-        <v>256</v>
+        <v>166</v>
       </c>
       <c r="E11">
-        <v>274</v>
+        <v>171</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>267</v>
+        <v>175.33333333333334</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>0.26700000000000002</v>
+        <v>0.17533333333333334</v>
       </c>
       <c r="H11" s="2">
-        <f>$H$28</f>
-        <v>0.10566666666666674</v>
+        <f>$H$32</f>
+        <v>5.3333333333333344E-2</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>0.16133333333333327</v>
+        <v>0.122</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C12">
-        <v>1258</v>
+        <v>1365</v>
       </c>
       <c r="D12">
-        <v>1301</v>
+        <v>1369</v>
       </c>
       <c r="E12">
-        <v>1393</v>
+        <v>1357</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>1317.3333333333333</v>
+        <v>1363.6666666666667</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.3173333333333332</v>
+        <v>1.3636666666666668</v>
       </c>
       <c r="H12" s="2">
-        <f>$H$28</f>
-        <v>0.10566666666666674</v>
+        <f>$H$32</f>
+        <v>5.3333333333333344E-2</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1.2116666666666664</v>
+        <v>1.3103333333333333</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>137</v>
+        <v>271</v>
       </c>
       <c r="D13">
-        <v>139</v>
+        <v>268</v>
       </c>
       <c r="E13">
-        <v>144</v>
+        <v>275</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>271.33333333333331</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>0.27133333333333332</v>
       </c>
       <c r="H13" s="2">
-        <f>$H$29</f>
-        <v>3.400000000000003E-2</v>
+        <f>$H$33</f>
+        <v>0.11899999999999994</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>0.10599999999999998</v>
+        <v>0.15233333333333338</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>1090</v>
+        <v>1290</v>
       </c>
       <c r="D14">
-        <v>1078</v>
+        <v>1285</v>
       </c>
       <c r="E14">
-        <v>1103</v>
+        <v>1264</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>1090.3333333333333</v>
+        <v>1279.6666666666667</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>1.0903333333333332</v>
+        <v>1.2796666666666667</v>
       </c>
       <c r="H14" s="2">
-        <f>$H$29</f>
-        <v>3.400000000000003E-2</v>
+        <f>$H$33</f>
+        <v>0.11899999999999994</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>1.0563333333333331</v>
+        <v>1.1606666666666667</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>11731</v>
+        <v>138</v>
       </c>
       <c r="D15">
-        <v>11755</v>
+        <v>141</v>
       </c>
       <c r="E15">
-        <v>11813</v>
+        <v>139</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>11766.333333333334</v>
+        <v>139.33333333333334</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>11.766333333333334</v>
+        <v>0.13933333333333334</v>
       </c>
       <c r="H15" s="2">
-        <f>$H$25</f>
-        <v>0.22633333333333328</v>
+        <f>$H$34</f>
+        <v>3.4333333333333327E-2</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>11.540000000000001</v>
+        <v>0.10500000000000001</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>14613</v>
+        <v>1070</v>
       </c>
       <c r="D16">
-        <v>14620</v>
+        <v>1115</v>
       </c>
       <c r="E16">
-        <v>14624</v>
+        <v>1109</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>14619</v>
+        <v>1098</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>14.619</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="H16" s="2">
-        <f>$H$25</f>
-        <v>0.22633333333333328</v>
+        <f>$H$34</f>
+        <v>3.4333333333333327E-2</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>14.392666666666667</v>
+        <v>1.0636666666666668</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>4660</v>
+        <v>11931</v>
       </c>
       <c r="D17">
-        <v>4666</v>
+        <v>11954</v>
       </c>
       <c r="E17">
-        <v>4645</v>
+        <v>11919</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>4657</v>
+        <v>11934.666666666666</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>4.657</v>
+        <v>11.934666666666667</v>
       </c>
       <c r="H17" s="2">
-        <f>$H$26</f>
-        <v>4.2333333333333306E-2</v>
+        <f>$H$29</f>
+        <v>0.22466666666666679</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>4.6146666666666665</v>
+        <v>11.71</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>7333</v>
+        <v>14744</v>
       </c>
       <c r="D18">
-        <v>7405</v>
+        <v>14827</v>
       </c>
       <c r="E18">
-        <v>7351</v>
+        <v>14868</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>7363</v>
+        <v>14813</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>7.3630000000000004</v>
+        <v>14.813000000000001</v>
       </c>
       <c r="H18" s="2">
-        <f>$H$26</f>
-        <v>4.2333333333333306E-2</v>
+        <f>$H$29</f>
+        <v>0.22466666666666679</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>7.3206666666666669</v>
+        <v>14.588333333333335</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C19">
-        <v>4720</v>
+        <v>5138</v>
       </c>
       <c r="D19">
-        <v>4725</v>
+        <v>5148</v>
       </c>
       <c r="E19">
-        <v>4769</v>
+        <v>5177</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>4738</v>
+        <v>5154.333333333333</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>4.7380000000000004</v>
+        <v>5.1543333333333328</v>
       </c>
       <c r="H19" s="2">
-        <f>$H$27</f>
-        <v>5.5999999999999994E-2</v>
+        <f>$H$30</f>
+        <v>0.13666666666666683</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>4.6820000000000004</v>
+        <v>5.0176666666666661</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C20">
-        <v>7670</v>
+        <v>7517</v>
       </c>
       <c r="D20">
-        <v>7662</v>
+        <v>7603</v>
       </c>
       <c r="E20">
-        <v>7639</v>
+        <v>7539</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>7657</v>
+        <v>7553</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>7.657</v>
+        <v>7.5529999999999999</v>
       </c>
       <c r="H20" s="2">
-        <f>$H$27</f>
-        <v>5.5999999999999994E-2</v>
+        <f>$H$30</f>
+        <v>0.13666666666666683</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>7.601</v>
+        <v>7.4163333333333332</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>5244</v>
+        <v>4646</v>
       </c>
       <c r="D21">
-        <v>5210</v>
+        <v>4669</v>
       </c>
       <c r="E21">
-        <v>5259</v>
+        <v>4681</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>5237.666666666667</v>
+        <v>4665.333333333333</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>5.2376666666666667</v>
+        <v>4.6653333333333329</v>
       </c>
       <c r="H21" s="2">
-        <f>$H$28</f>
-        <v>0.10566666666666674</v>
+        <f>$H$31</f>
+        <v>4.6666666666666662E-2</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>5.1319999999999997</v>
+        <v>4.618666666666666</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>7925</v>
+        <v>7379</v>
       </c>
       <c r="D22">
-        <v>7945</v>
+        <v>7449</v>
       </c>
       <c r="E22">
-        <v>7895</v>
+        <v>7433</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>7921.666666666667</v>
+        <v>7420.333333333333</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>7.9216666666666669</v>
+        <v>7.4203333333333328</v>
       </c>
       <c r="H22" s="2">
-        <f>$H$28</f>
-        <v>0.10566666666666674</v>
+        <f>$H$31</f>
+        <v>4.6666666666666662E-2</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>7.8159999999999998</v>
+        <v>7.3736666666666659</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>4707</v>
+        <v>4739</v>
       </c>
       <c r="D23">
-        <v>4683</v>
+        <v>4779</v>
       </c>
       <c r="E23">
-        <v>4685</v>
+        <v>4763</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>4691.666666666667</v>
+        <v>4760.333333333333</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>4.6916666666666673</v>
+        <v>4.7603333333333326</v>
       </c>
       <c r="H23" s="2">
-        <f>$H$29</f>
-        <v>3.400000000000003E-2</v>
+        <f>$H$32</f>
+        <v>5.3333333333333344E-2</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>4.6576666666666675</v>
+        <v>4.706999999999999</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C24">
-        <v>7360</v>
+        <v>7656</v>
       </c>
       <c r="D24">
-        <v>7406</v>
+        <v>7729</v>
       </c>
       <c r="E24">
-        <v>7378</v>
+        <v>7681</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>7381.333333333333</v>
+        <v>7688.666666666667</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>7.3813333333333331</v>
+        <v>7.6886666666666672</v>
       </c>
       <c r="H24" s="2">
-        <f>$H$29</f>
-        <v>3.400000000000003E-2</v>
+        <f>$H$32</f>
+        <v>5.3333333333333344E-2</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>7.3473333333333333</v>
+        <v>7.6353333333333335</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>1471</v>
+        <v>5206</v>
       </c>
       <c r="D25">
-        <v>1504</v>
+        <v>5259</v>
       </c>
       <c r="E25">
-        <v>1476</v>
+        <v>5240</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>1483.6666666666667</v>
+        <v>5235</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>1.4836666666666667</v>
-      </c>
-      <c r="H25" s="3">
-        <f>2*G5-G25</f>
-        <v>0.22633333333333328</v>
+        <v>5.2350000000000003</v>
+      </c>
+      <c r="H25" s="2">
+        <f>$H$33</f>
+        <v>0.11899999999999994</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>5.1160000000000005</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>234</v>
+        <v>8077</v>
       </c>
       <c r="D26">
-        <v>254</v>
+        <v>8012</v>
       </c>
       <c r="E26">
-        <v>243</v>
+        <v>8109</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>243.66666666666666</v>
+        <v>8066</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>0.24366666666666667</v>
-      </c>
-      <c r="H26" s="3">
-        <f>2*G7-G26</f>
-        <v>4.2333333333333306E-2</v>
+        <v>8.0660000000000007</v>
+      </c>
+      <c r="H26" s="2">
+        <f>$H$33</f>
+        <v>0.11899999999999994</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>7.947000000000001</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27">
-        <v>291</v>
+        <v>4702</v>
       </c>
       <c r="D27">
-        <v>285</v>
+        <v>4717</v>
       </c>
       <c r="E27">
-        <v>310</v>
+        <v>4794</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>295.33333333333331</v>
+        <v>4737.666666666667</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>0.29533333333333334</v>
-      </c>
-      <c r="H27" s="3">
-        <f>2*G9-G27</f>
-        <v>5.5999999999999994E-2</v>
+        <v>4.7376666666666667</v>
+      </c>
+      <c r="H27" s="2">
+        <f>$H$34</f>
+        <v>3.4333333333333327E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>4.7033333333333331</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>416</v>
+        <v>7478</v>
       </c>
       <c r="D28">
-        <v>423</v>
+        <v>7445</v>
       </c>
       <c r="E28">
-        <v>446</v>
+        <v>7505</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>428.33333333333331</v>
+        <v>7476</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>0.42833333333333329</v>
-      </c>
-      <c r="H28" s="3">
-        <f>2*G11-G28</f>
-        <v>0.10566666666666674</v>
+        <v>7.476</v>
+      </c>
+      <c r="H28" s="2">
+        <f>$H$34</f>
+        <v>3.4333333333333327E-2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>7.4416666666666664</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>1388</v>
+      </c>
+      <c r="D29">
+        <v>1529</v>
+      </c>
+      <c r="E29">
+        <v>1511</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>1476</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1.476</v>
+      </c>
+      <c r="H29" s="3">
+        <f>2*G5-G29</f>
+        <v>0.22466666666666679</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>628</v>
+      </c>
+      <c r="D30">
+        <v>613</v>
+      </c>
+      <c r="E30">
+        <v>621</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>620.66666666666663</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0.62066666666666659</v>
+      </c>
+      <c r="H30" s="3">
+        <f>2*G7-G30</f>
+        <v>0.13666666666666683</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>242</v>
+      </c>
+      <c r="D31">
+        <v>235</v>
+      </c>
+      <c r="E31">
+        <v>239</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>238.66666666666666</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.23866666666666667</v>
+      </c>
+      <c r="H31" s="3">
+        <f>2*G9-G31</f>
+        <v>4.6666666666666662E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>293</v>
+      </c>
+      <c r="D32">
+        <v>310</v>
+      </c>
+      <c r="E32">
+        <v>289</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>297.33333333333331</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.29733333333333334</v>
+      </c>
+      <c r="H32" s="3">
+        <f>2*G11-G32</f>
+        <v>5.3333333333333344E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33">
+        <v>417</v>
+      </c>
+      <c r="D33">
+        <v>403</v>
+      </c>
+      <c r="E33">
+        <v>451</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>423.66666666666669</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.42366666666666669</v>
+      </c>
+      <c r="H33" s="3">
+        <f>2*G13-G33</f>
+        <v>0.11899999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>238</v>
-      </c>
-      <c r="D29">
-        <v>257</v>
-      </c>
-      <c r="E29">
-        <v>243</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="0"/>
-        <v>246</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="1"/>
-        <v>0.246</v>
-      </c>
-      <c r="H29" s="3">
-        <f>2*G13-G29</f>
-        <v>3.400000000000003E-2</v>
+      <c r="C34">
+        <v>239</v>
+      </c>
+      <c r="D34">
+        <v>245</v>
+      </c>
+      <c r="E34">
+        <v>249</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>244.33333333333334</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.24433333333333335</v>
+      </c>
+      <c r="H34" s="3">
+        <f>2*G15-G34</f>
+        <v>3.4333333333333327E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>